<commit_message>
Corrected power conversion inversion
</commit_message>
<xml_diff>
--- a/kb/unit-converter/power.xlsx
+++ b/kb/unit-converter/power.xlsx
@@ -291,7 +291,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,8 +366,8 @@
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>0.7457</v>
+      <c r="B7" s="0" t="n">
+        <v>1.3410218586563</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>14</v>

</xml_diff>